<commit_message>
Changed the likelihood function
</commit_message>
<xml_diff>
--- a/results/example2/mcmc_summary.xlsx
+++ b/results/example2/mcmc_summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Run_Index</t>
   </si>
@@ -428,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -814,6 +814,333 @@
         <v>0.001</v>
       </c>
     </row>
+    <row r="8" spans="1:18">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>277</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1.984147416992253</v>
+      </c>
+      <c r="G8">
+        <v>1.094185742614283</v>
+      </c>
+      <c r="H8">
+        <v>-4.054140384558921E+18</v>
+      </c>
+      <c r="I8">
+        <v>-0.4196813310094601</v>
+      </c>
+      <c r="J8">
+        <v>0.1037613926518594</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>4.348552697956077</v>
+      </c>
+      <c r="M8">
+        <v>0.05776494112419462</v>
+      </c>
+      <c r="N8">
+        <v>1.047036280321465</v>
+      </c>
+      <c r="O8">
+        <v>4501</v>
+      </c>
+      <c r="P8">
+        <v>50000</v>
+      </c>
+      <c r="Q8">
+        <v>100</v>
+      </c>
+      <c r="R8">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>277</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0.02728044638051733</v>
+      </c>
+      <c r="G9">
+        <v>0.1218393006309193</v>
+      </c>
+      <c r="H9">
+        <v>1919392285086128</v>
+      </c>
+      <c r="I9">
+        <v>1.981140093966673</v>
+      </c>
+      <c r="J9">
+        <v>0.3443625851306916</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0.4724485237261105</v>
+      </c>
+      <c r="M9">
+        <v>0.941124194623417</v>
+      </c>
+      <c r="N9">
+        <v>1.047036280321465</v>
+      </c>
+      <c r="O9">
+        <v>4501</v>
+      </c>
+      <c r="P9">
+        <v>50000</v>
+      </c>
+      <c r="Q9">
+        <v>100</v>
+      </c>
+      <c r="R9">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>277</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1.35636303285016</v>
+      </c>
+      <c r="G10">
+        <v>0.0884353397009327</v>
+      </c>
+      <c r="H10">
+        <v>1.192394230752624E+18</v>
+      </c>
+      <c r="I10">
+        <v>0.1002633741811969</v>
+      </c>
+      <c r="J10">
+        <v>0.009326608762688406</v>
+      </c>
+      <c r="K10">
+        <v>1.183656053444713</v>
+      </c>
+      <c r="L10">
+        <v>1.537357355969161</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>1.047036280321465</v>
+      </c>
+      <c r="O10">
+        <v>4501</v>
+      </c>
+      <c r="P10">
+        <v>50000</v>
+      </c>
+      <c r="Q10">
+        <v>100</v>
+      </c>
+      <c r="R10">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>146</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1.322248709008332</v>
+      </c>
+      <c r="G11">
+        <v>0.3016152184436793</v>
+      </c>
+      <c r="H11">
+        <v>1.689225160232883E+18</v>
+      </c>
+      <c r="I11">
+        <v>-1.731494958368718</v>
+      </c>
+      <c r="J11">
+        <v>0.5647020392356592</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>1.614184578823112</v>
+      </c>
+      <c r="M11">
+        <v>0.04287936014219063</v>
+      </c>
+      <c r="N11">
+        <v>1.325190999290214</v>
+      </c>
+      <c r="O11">
+        <v>4501</v>
+      </c>
+      <c r="P11">
+        <v>50000</v>
+      </c>
+      <c r="Q11">
+        <v>100</v>
+      </c>
+      <c r="R11">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>146</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0.1</v>
+      </c>
+      <c r="F12">
+        <v>0.01174165124139144</v>
+      </c>
+      <c r="G12">
+        <v>0.05555521182835848</v>
+      </c>
+      <c r="H12">
+        <v>2129275412058256</v>
+      </c>
+      <c r="I12">
+        <v>1.883987746387548</v>
+      </c>
+      <c r="J12">
+        <v>0.6297939731774923</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0.270295874176763</v>
+      </c>
+      <c r="M12">
+        <v>0.9568984670073317</v>
+      </c>
+      <c r="N12">
+        <v>1.325190999290214</v>
+      </c>
+      <c r="O12">
+        <v>4501</v>
+      </c>
+      <c r="P12">
+        <v>50000</v>
+      </c>
+      <c r="Q12">
+        <v>100</v>
+      </c>
+      <c r="R12">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>146</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1.325190999290214</v>
+      </c>
+      <c r="O13">
+        <v>4501</v>
+      </c>
+      <c r="P13">
+        <v>50000</v>
+      </c>
+      <c r="Q13">
+        <v>100</v>
+      </c>
+      <c r="R13">
+        <v>0.001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>